<commit_message>
made changes to gantt chart
</commit_message>
<xml_diff>
--- a/docs/Gantt.xlsx
+++ b/docs/Gantt.xlsx
@@ -898,6 +898,36 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="12">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="10" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="10" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -905,36 +935,6 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="11" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="10" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="10" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1200,7 +1200,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8638EF3-2DAE-40BC-A45A-2B8C536FAB0D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8638EF3-2DAE-40BC-A45A-2B8C536FAB0D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1490,7 +1490,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1504,8 +1504,8 @@
   <dimension ref="A1:BL36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BO13" sqref="BO13"/>
+      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1543,7 +1543,7 @@
       <c r="B2" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="91"/>
+      <c r="E2" s="84"/>
       <c r="I2" s="61"/>
     </row>
     <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1553,118 +1553,118 @@
       <c r="B3" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="83" t="s">
+      <c r="C3" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="84"/>
-      <c r="E3" s="89">
+      <c r="D3" s="94"/>
+      <c r="E3" s="92">
         <f>DATE(2019,10,1)</f>
         <v>43739</v>
       </c>
-      <c r="F3" s="89"/>
+      <c r="F3" s="92"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="83" t="s">
+      <c r="C4" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="84"/>
+      <c r="D4" s="94"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="86">
+      <c r="I4" s="89">
         <f>I5</f>
         <v>43738</v>
       </c>
-      <c r="J4" s="87"/>
-      <c r="K4" s="87"/>
-      <c r="L4" s="87"/>
-      <c r="M4" s="87"/>
-      <c r="N4" s="87"/>
-      <c r="O4" s="88"/>
-      <c r="P4" s="86">
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="90"/>
+      <c r="O4" s="91"/>
+      <c r="P4" s="89">
         <f>P5</f>
         <v>43745</v>
       </c>
-      <c r="Q4" s="87"/>
-      <c r="R4" s="87"/>
-      <c r="S4" s="87"/>
-      <c r="T4" s="87"/>
-      <c r="U4" s="87"/>
-      <c r="V4" s="88"/>
-      <c r="W4" s="86">
+      <c r="Q4" s="90"/>
+      <c r="R4" s="90"/>
+      <c r="S4" s="90"/>
+      <c r="T4" s="90"/>
+      <c r="U4" s="90"/>
+      <c r="V4" s="91"/>
+      <c r="W4" s="89">
         <f>W5</f>
         <v>43752</v>
       </c>
-      <c r="X4" s="87"/>
-      <c r="Y4" s="87"/>
-      <c r="Z4" s="87"/>
-      <c r="AA4" s="87"/>
-      <c r="AB4" s="87"/>
-      <c r="AC4" s="88"/>
-      <c r="AD4" s="86">
+      <c r="X4" s="90"/>
+      <c r="Y4" s="90"/>
+      <c r="Z4" s="90"/>
+      <c r="AA4" s="90"/>
+      <c r="AB4" s="90"/>
+      <c r="AC4" s="91"/>
+      <c r="AD4" s="89">
         <f>AD5</f>
         <v>43759</v>
       </c>
-      <c r="AE4" s="87"/>
-      <c r="AF4" s="87"/>
-      <c r="AG4" s="87"/>
-      <c r="AH4" s="87"/>
-      <c r="AI4" s="87"/>
-      <c r="AJ4" s="88"/>
-      <c r="AK4" s="86">
+      <c r="AE4" s="90"/>
+      <c r="AF4" s="90"/>
+      <c r="AG4" s="90"/>
+      <c r="AH4" s="90"/>
+      <c r="AI4" s="90"/>
+      <c r="AJ4" s="91"/>
+      <c r="AK4" s="89">
         <f>AK5</f>
         <v>43766</v>
       </c>
-      <c r="AL4" s="87"/>
-      <c r="AM4" s="87"/>
-      <c r="AN4" s="87"/>
-      <c r="AO4" s="87"/>
-      <c r="AP4" s="87"/>
-      <c r="AQ4" s="88"/>
-      <c r="AR4" s="86">
+      <c r="AL4" s="90"/>
+      <c r="AM4" s="90"/>
+      <c r="AN4" s="90"/>
+      <c r="AO4" s="90"/>
+      <c r="AP4" s="90"/>
+      <c r="AQ4" s="91"/>
+      <c r="AR4" s="89">
         <f>AR5</f>
         <v>43773</v>
       </c>
-      <c r="AS4" s="87"/>
-      <c r="AT4" s="87"/>
-      <c r="AU4" s="87"/>
-      <c r="AV4" s="87"/>
-      <c r="AW4" s="87"/>
-      <c r="AX4" s="88"/>
-      <c r="AY4" s="86">
+      <c r="AS4" s="90"/>
+      <c r="AT4" s="90"/>
+      <c r="AU4" s="90"/>
+      <c r="AV4" s="90"/>
+      <c r="AW4" s="90"/>
+      <c r="AX4" s="91"/>
+      <c r="AY4" s="89">
         <f>AY5</f>
         <v>43780</v>
       </c>
-      <c r="AZ4" s="87"/>
-      <c r="BA4" s="87"/>
-      <c r="BB4" s="87"/>
-      <c r="BC4" s="87"/>
-      <c r="BD4" s="87"/>
-      <c r="BE4" s="88"/>
-      <c r="BF4" s="86">
+      <c r="AZ4" s="90"/>
+      <c r="BA4" s="90"/>
+      <c r="BB4" s="90"/>
+      <c r="BC4" s="90"/>
+      <c r="BD4" s="90"/>
+      <c r="BE4" s="91"/>
+      <c r="BF4" s="89">
         <f>BF5</f>
         <v>43787</v>
       </c>
-      <c r="BG4" s="87"/>
-      <c r="BH4" s="87"/>
-      <c r="BI4" s="87"/>
-      <c r="BJ4" s="87"/>
-      <c r="BK4" s="87"/>
-      <c r="BL4" s="88"/>
+      <c r="BG4" s="90"/>
+      <c r="BH4" s="90"/>
+      <c r="BI4" s="90"/>
+      <c r="BJ4" s="90"/>
+      <c r="BK4" s="90"/>
+      <c r="BL4" s="91"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="85"/>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="85"/>
+      <c r="B5" s="95"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="95"/>
       <c r="I5" s="11">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43738</v>
@@ -2282,10 +2282,10 @@
       <c r="A9" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="90" t="s">
+      <c r="B9" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="92" t="s">
+      <c r="C9" s="85" t="s">
         <v>49</v>
       </c>
       <c r="D9" s="22">
@@ -2365,7 +2365,7 @@
       <c r="A10" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="90" t="s">
+      <c r="B10" s="83" t="s">
         <v>51</v>
       </c>
       <c r="C10" s="71"/>
@@ -2444,7 +2444,7 @@
     </row>
     <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="58"/>
-      <c r="B11" s="90" t="s">
+      <c r="B11" s="83" t="s">
         <v>53</v>
       </c>
       <c r="C11" s="71"/>
@@ -2523,7 +2523,7 @@
     </row>
     <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="58"/>
-      <c r="B12" s="90" t="s">
+      <c r="B12" s="83" t="s">
         <v>54</v>
       </c>
       <c r="C12" s="71"/>
@@ -2602,12 +2602,12 @@
     </row>
     <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="58"/>
-      <c r="B13" s="90" t="s">
+      <c r="B13" s="83" t="s">
         <v>55</v>
       </c>
       <c r="C13" s="71"/>
       <c r="D13" s="22">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="E13" s="66">
         <f>E10+15</f>
@@ -2754,7 +2754,7 @@
     </row>
     <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="59"/>
-      <c r="B15" s="93" t="s">
+      <c r="B15" s="86" t="s">
         <v>57</v>
       </c>
       <c r="C15" s="73"/>
@@ -2833,18 +2833,18 @@
     </row>
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="58"/>
-      <c r="B16" s="93" t="s">
+      <c r="B16" s="86" t="s">
         <v>58</v>
       </c>
       <c r="C16" s="73"/>
       <c r="D16" s="27">
         <v>0.3</v>
       </c>
-      <c r="E16" s="94">
+      <c r="E16" s="87">
         <f>E15</f>
         <v>43764</v>
       </c>
-      <c r="F16" s="94">
+      <c r="F16" s="87">
         <f>E16+4</f>
         <v>43768</v>
       </c>
@@ -2917,10 +2917,10 @@
       </c>
       <c r="C17" s="73"/>
       <c r="D17" s="27"/>
-      <c r="E17" s="94" t="s">
+      <c r="E17" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="94" t="s">
+      <c r="F17" s="87" t="s">
         <v>34</v>
       </c>
       <c r="G17" s="17"/>
@@ -2992,10 +2992,10 @@
       </c>
       <c r="C18" s="73"/>
       <c r="D18" s="27"/>
-      <c r="E18" s="94" t="s">
+      <c r="E18" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="94" t="s">
+      <c r="F18" s="87" t="s">
         <v>34</v>
       </c>
       <c r="G18" s="17"/>
@@ -3067,10 +3067,10 @@
       </c>
       <c r="C19" s="73"/>
       <c r="D19" s="27"/>
-      <c r="E19" s="94" t="s">
+      <c r="E19" s="87" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="94" t="s">
+      <c r="F19" s="87" t="s">
         <v>34</v>
       </c>
       <c r="G19" s="17"/>
@@ -3215,10 +3215,10 @@
       </c>
       <c r="C21" s="75"/>
       <c r="D21" s="32"/>
-      <c r="E21" s="95" t="s">
+      <c r="E21" s="88" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="95" t="s">
+      <c r="F21" s="88" t="s">
         <v>34</v>
       </c>
       <c r="G21" s="17"/>
@@ -3290,10 +3290,10 @@
       </c>
       <c r="C22" s="75"/>
       <c r="D22" s="32"/>
-      <c r="E22" s="95" t="s">
+      <c r="E22" s="88" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="95" t="s">
+      <c r="F22" s="88" t="s">
         <v>34</v>
       </c>
       <c r="G22" s="17"/>
@@ -3365,10 +3365,10 @@
       </c>
       <c r="C23" s="75"/>
       <c r="D23" s="32"/>
-      <c r="E23" s="95" t="s">
+      <c r="E23" s="88" t="s">
         <v>34</v>
       </c>
-      <c r="F23" s="95" t="s">
+      <c r="F23" s="88" t="s">
         <v>34</v>
       </c>
       <c r="G23" s="17"/>
@@ -3440,10 +3440,10 @@
       </c>
       <c r="C24" s="75"/>
       <c r="D24" s="32"/>
-      <c r="E24" s="95" t="s">
+      <c r="E24" s="88" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="95" t="s">
+      <c r="F24" s="88" t="s">
         <v>34</v>
       </c>
       <c r="G24" s="17"/>
@@ -3515,10 +3515,10 @@
       </c>
       <c r="C25" s="75"/>
       <c r="D25" s="32"/>
-      <c r="E25" s="95" t="s">
+      <c r="E25" s="88" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="95" t="s">
+      <c r="F25" s="88" t="s">
         <v>34</v>
       </c>
       <c r="G25" s="17"/>
@@ -4187,6 +4187,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4194,11 +4199,6 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D33">
     <cfRule type="dataBar" priority="14">

</xml_diff>